<commit_message>
adding more tests and functionality for cell values other than strings
</commit_message>
<xml_diff>
--- a/specs/data/simple_with_picture.xlsx
+++ b/specs/data/simple_with_picture.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="21080" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="text &amp; pic" sheetId="1" r:id="rId1"/>
+    <sheet name="numbers" sheetId="2" r:id="rId2"/>
+    <sheet name="dates" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>This</t>
   </si>
@@ -34,20 +39,72 @@
   </si>
   <si>
     <t>workbook</t>
+  </si>
+  <si>
+    <t>NUM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQUARE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUBE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQUARE ROOT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>m/dd/yy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy-mm-dd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMM dd, yyyy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Monaco"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,14 +127,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -410,14 +472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -450,31 +512,553 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2*A2</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>B2*A2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>SQRT(A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B16" si="0">A3*A3</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C16" si="1">B3*A3</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="2">SQRT(A3)</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>1.7320508075688772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>343</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>2.6457513110645907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>2.8284271247461903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>729</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>3.1622776601683795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>1331</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>3.3166247903553998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>1728</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>3.4641016151377544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2197</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>3.6055512754639891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>2744</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>3.7416573867739413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>3375</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>3.872983346207417</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>40237</v>
+      </c>
+      <c r="B2" s="4">
+        <f>A16</f>
+        <v>40251</v>
+      </c>
+      <c r="C2" s="5">
+        <f>B16</f>
+        <v>40265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <f>A2+1</f>
+        <v>40238</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B2+1</f>
+        <v>40252</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:C16" si="0">C2+1</f>
+        <v>40266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A16" si="1">A3+1</f>
+        <v>40239</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B16" si="2">B3+1</f>
+        <v>40253</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" si="0"/>
+        <v>40267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <f t="shared" si="1"/>
+        <v>40240</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="2"/>
+        <v>40254</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" si="0"/>
+        <v>40268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <f t="shared" si="1"/>
+        <v>40241</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="2"/>
+        <v>40255</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" si="0"/>
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <f t="shared" si="1"/>
+        <v>40242</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="2"/>
+        <v>40256</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>40270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>40243</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="2"/>
+        <v>40257</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>40271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>40244</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="2"/>
+        <v>40258</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>40272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>40245</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="2"/>
+        <v>40259</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>40273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>40246</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="2"/>
+        <v>40260</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>40274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>40247</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="2"/>
+        <v>40261</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>40275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>40248</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="2"/>
+        <v>40262</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>40276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>40249</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="2"/>
+        <v>40263</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>40277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>40250</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="2"/>
+        <v>40264</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>40278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>40251</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="2"/>
+        <v>40265</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>40279</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>